<commit_message>
Revert "Updated upload template"
This reverts commit b651d0b6aed9399bc4cd3f91362d9c31988cdcd2.
</commit_message>
<xml_diff>
--- a/Client Avails Upload Template.xlsx
+++ b/Client Avails Upload Template.xlsx
@@ -12,14 +12,14 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$1:$Z$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$2:$Y$4</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="43">
   <si>
     <t>Video Version</t>
   </si>
@@ -148,30 +148,15 @@
   </si>
   <si>
     <t>Optional - Formula</t>
-  </si>
-  <si>
-    <t>Announce Override</t>
-  </si>
-  <si>
-    <t>Vendor ID</t>
-  </si>
-  <si>
-    <t>Title Name</t>
-  </si>
-  <si>
-    <t>Dummy, Title</t>
-  </si>
-  <si>
-    <t>Dummy, Title1</t>
-  </si>
-  <si>
-    <t>Suppress</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
+  </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -656,8 +641,8 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1001,471 +986,440 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:AC4"/>
+  <dimension ref="A1:Y4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="26.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="22" max="23" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="L1" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="M1" s="5" t="s">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="L1" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="M1" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="O1" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="P1" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q1" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="R1" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="S1" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="T1" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="U1" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="V1" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="W1" s="5" t="s">
+      <c r="N1" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="O1" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="P1" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q1" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="R1" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="S1" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="T1" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="U1" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="V1" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="X1" s="5" t="s">
+      <c r="W1" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="Y1" s="5" t="s">
+      <c r="X1" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="Z1" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="AA1" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="AB1" s="5" t="s">
+      <c r="Y1" s="6" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>45</v>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>6000000001</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H3" s="5">
+        <v>41856</v>
+      </c>
+      <c r="I3" s="5">
+        <v>54788</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="L3" s="4">
+        <v>111</v>
+      </c>
+      <c r="M3" s="4">
+        <v>1.9</v>
+      </c>
+      <c r="N3" s="4">
+        <v>2.99</v>
+      </c>
+      <c r="O3" s="4">
         <v>1</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="R2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="S2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="T2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="U2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="V2" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="W2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="X2" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="Y2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="Z2" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="AA2" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AB2" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B3" s="1">
-        <v>6000000001</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="I3" s="2">
-        <v>42522</v>
-      </c>
-      <c r="J3" s="2">
-        <v>54788</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="M3" s="4">
-        <v>111</v>
-      </c>
-      <c r="N3" s="4"/>
-      <c r="O3" s="4"/>
-      <c r="P3" s="4"/>
+      <c r="P3" s="4">
+        <v>1.99</v>
+      </c>
       <c r="Q3" s="4">
         <v>1.99</v>
       </c>
-      <c r="R3" s="4">
+      <c r="R3" s="5"/>
+      <c r="S3" s="5"/>
+      <c r="T3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="U3" s="3">
+        <v>883316107812</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="W3" s="1">
+        <v>5</v>
+      </c>
+      <c r="X3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y3" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>6000000002</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H4" s="5">
+        <v>41856</v>
+      </c>
+      <c r="I4" s="5">
+        <v>43800</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="L4" s="4">
+        <v>111</v>
+      </c>
+      <c r="M4" s="4">
+        <v>1.9</v>
+      </c>
+      <c r="N4" s="4">
+        <v>2.99</v>
+      </c>
+      <c r="O4" s="4">
+        <v>1</v>
+      </c>
+      <c r="P4" s="4">
         <v>1.99</v>
       </c>
-      <c r="S3" s="2">
-        <v>42522</v>
-      </c>
-      <c r="T3" s="2">
-        <v>42522</v>
-      </c>
-      <c r="U3" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="V3" s="3">
-        <v>883316107812</v>
-      </c>
-      <c r="W3" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="X3" s="1">
-        <v>5</v>
-      </c>
-      <c r="Y3" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="Z3" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="AA3" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="AC3" s="5"/>
-    </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B4" s="1">
-        <v>6000000002</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="I4" s="2">
-        <v>42522</v>
-      </c>
-      <c r="J4" s="2">
-        <v>54788</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="M4" s="4">
-        <v>111</v>
-      </c>
-      <c r="N4" s="4"/>
-      <c r="O4" s="4"/>
-      <c r="P4" s="4"/>
       <c r="Q4" s="4">
         <v>1.99</v>
       </c>
-      <c r="R4" s="4">
-        <v>1.99</v>
-      </c>
-      <c r="S4" s="2">
-        <v>42522</v>
-      </c>
-      <c r="T4" s="2">
-        <v>42522</v>
-      </c>
-      <c r="U4" s="1" t="s">
+      <c r="R4" s="5"/>
+      <c r="S4" s="5"/>
+      <c r="T4" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="V4" s="3">
+      <c r="U4" s="3">
         <v>883316116289</v>
       </c>
-      <c r="W4" s="1" t="s">
+      <c r="V4" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="X4" s="1">
+      <c r="W4" s="1">
         <v>5</v>
       </c>
+      <c r="X4" s="1" t="s">
+        <v>37</v>
+      </c>
       <c r="Y4" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="Z4" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="AA4" s="1"/>
-      <c r="AB4">
-        <v>123</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
+  <dataValidations count="3">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2">
+      <formula1>"YYYY-MM-DD"</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Date format must be YYYY-MM-DD" error="Date format must be YYYY-MM-DD" promptTitle="Date format must be YYYY-MM-DD" prompt="Date format must be YYYY-MM-DD" sqref="H3:H1048576">
+      <formula1>"YYYY-MM-DD"</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Date Format must be YYYY-MM-DD" error="Date Format must be YYYY-MM-DD" promptTitle="Date Format must be YYYY-MM-DD" prompt="Date Format must be YYYY-MM-DD" sqref="I3:I1048576 R3:R1048576 S3:S1048576">
       <formula1>"YYYY-MM-DD"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="200" r:id="rId1"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:Y5"/>
+  <dimension ref="A1:Y1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="L1" s="5" t="s">
+      <c r="A1" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="L1" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="M1" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="N1" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="O1" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="P1" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q1" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="R1" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="S1" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="T1" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="U1" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="V1" s="5" t="s">
+      <c r="N1" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="O1" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="P1" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q1" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="R1" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="S1" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="T1" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="U1" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="V1" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="W1" s="5" t="s">
+      <c r="W1" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="X1" s="5" t="s">
+      <c r="X1" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="Y1" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A5" s="6">
-        <v>42984</v>
+      <c r="Y1" s="6" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "Revert "Updated upload template""
This reverts commit f471a28eacdc142ca92ed3c25b7f402c17455f45.
</commit_message>
<xml_diff>
--- a/Client Avails Upload Template.xlsx
+++ b/Client Avails Upload Template.xlsx
@@ -12,14 +12,14 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$2:$Y$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$1:$Z$4</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="49">
   <si>
     <t>Video Version</t>
   </si>
@@ -148,15 +148,30 @@
   </si>
   <si>
     <t>Optional - Formula</t>
+  </si>
+  <si>
+    <t>Announce Override</t>
+  </si>
+  <si>
+    <t>Vendor ID</t>
+  </si>
+  <si>
+    <t>Title Name</t>
+  </si>
+  <si>
+    <t>Dummy, Title</t>
+  </si>
+  <si>
+    <t>Dummy, Title1</t>
+  </si>
+  <si>
+    <t>Suppress</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
-  </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -641,8 +656,8 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -986,440 +1001,471 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:Y4"/>
+  <dimension ref="A1:AC4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="26.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="21" max="22" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="K1" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="L1" s="6" t="s">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="M1" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="N1" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="N1" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="O1" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="P1" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q1" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="R1" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="S1" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="T1" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="U1" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="V1" s="6" t="s">
+      <c r="O1" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="R1" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="S1" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="T1" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="U1" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="V1" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="W1" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="W1" s="6" t="s">
+      <c r="X1" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="X1" s="6" t="s">
+      <c r="Y1" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="Y1" s="6" t="s">
+      <c r="Z1" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="AA1" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="AB1" s="5" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="O2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="Q2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="R2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="S2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S2" s="1" t="s">
+      <c r="T2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T2" s="1" t="s">
+      <c r="U2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U2" s="3" t="s">
+      <c r="V2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="V2" s="1" t="s">
+      <c r="W2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="W2" s="1" t="s">
+      <c r="X2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="X2" s="1" t="s">
+      <c r="Y2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Y2" s="1" t="s">
+      <c r="Z2" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="AA2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>44</v>
+      </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" s="1">
         <v>6000000001</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="H3" s="5">
-        <v>41856</v>
-      </c>
-      <c r="I3" s="5">
+      <c r="I3" s="2">
+        <v>42522</v>
+      </c>
+      <c r="J3" s="2">
         <v>54788</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="L3" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="L3" s="4">
+      <c r="M3" s="4">
         <v>111</v>
       </c>
-      <c r="M3" s="4">
-        <v>1.9</v>
-      </c>
-      <c r="N3" s="4">
-        <v>2.99</v>
-      </c>
-      <c r="O3" s="4">
-        <v>1</v>
-      </c>
-      <c r="P3" s="4">
-        <v>1.99</v>
-      </c>
+      <c r="N3" s="4"/>
+      <c r="O3" s="4"/>
+      <c r="P3" s="4"/>
       <c r="Q3" s="4">
         <v>1.99</v>
       </c>
-      <c r="R3" s="5"/>
-      <c r="S3" s="5"/>
-      <c r="T3" s="1" t="s">
+      <c r="R3" s="4">
+        <v>1.99</v>
+      </c>
+      <c r="S3" s="2">
+        <v>42522</v>
+      </c>
+      <c r="T3" s="2">
+        <v>42522</v>
+      </c>
+      <c r="U3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="U3" s="3">
+      <c r="V3" s="3">
         <v>883316107812</v>
       </c>
-      <c r="V3" s="1" t="s">
+      <c r="W3" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="W3" s="1">
+      <c r="X3" s="1">
         <v>5</v>
       </c>
-      <c r="X3" s="1" t="s">
+      <c r="Y3" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="Y3" s="1" t="s">
+      <c r="Z3" s="1" t="s">
         <v>33</v>
       </c>
+      <c r="AA3" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC3" s="5"/>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" s="1">
         <v>6000000002</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="H4" s="5">
-        <v>41856</v>
-      </c>
-      <c r="I4" s="5">
-        <v>43800</v>
-      </c>
-      <c r="J4" s="1" t="s">
+      <c r="I4" s="2">
+        <v>42522</v>
+      </c>
+      <c r="J4" s="2">
+        <v>54788</v>
+      </c>
+      <c r="K4" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="L4" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="L4" s="4">
+      <c r="M4" s="4">
         <v>111</v>
       </c>
-      <c r="M4" s="4">
-        <v>1.9</v>
-      </c>
-      <c r="N4" s="4">
-        <v>2.99</v>
-      </c>
-      <c r="O4" s="4">
-        <v>1</v>
-      </c>
-      <c r="P4" s="4">
-        <v>1.99</v>
-      </c>
+      <c r="N4" s="4"/>
+      <c r="O4" s="4"/>
+      <c r="P4" s="4"/>
       <c r="Q4" s="4">
         <v>1.99</v>
       </c>
-      <c r="R4" s="5"/>
-      <c r="S4" s="5"/>
-      <c r="T4" s="1" t="s">
+      <c r="R4" s="4">
+        <v>1.99</v>
+      </c>
+      <c r="S4" s="2">
+        <v>42522</v>
+      </c>
+      <c r="T4" s="2">
+        <v>42522</v>
+      </c>
+      <c r="U4" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="U4" s="3">
+      <c r="V4" s="3">
         <v>883316116289</v>
       </c>
-      <c r="V4" s="1" t="s">
+      <c r="W4" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="W4" s="1">
+      <c r="X4" s="1">
         <v>5</v>
       </c>
-      <c r="X4" s="1" t="s">
+      <c r="Y4" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="Y4" s="1" t="s">
+      <c r="Z4" s="1" t="s">
         <v>33</v>
+      </c>
+      <c r="AA4" s="1"/>
+      <c r="AB4">
+        <v>123</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="3">
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2">
-      <formula1>"YYYY-MM-DD"</formula1>
-    </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Date format must be YYYY-MM-DD" error="Date format must be YYYY-MM-DD" promptTitle="Date format must be YYYY-MM-DD" prompt="Date format must be YYYY-MM-DD" sqref="H3:H1048576">
-      <formula1>"YYYY-MM-DD"</formula1>
-    </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Date Format must be YYYY-MM-DD" error="Date Format must be YYYY-MM-DD" promptTitle="Date Format must be YYYY-MM-DD" prompt="Date Format must be YYYY-MM-DD" sqref="I3:I1048576 R3:R1048576 S3:S1048576">
+  <dataValidations count="1">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
       <formula1>"YYYY-MM-DD"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" verticalDpi="200" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:Y1"/>
+  <dimension ref="A1:Y5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="K1" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="L1" s="6" t="s">
+      <c r="A1" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="L1" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="M1" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="N1" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="O1" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="P1" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q1" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="R1" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="S1" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="T1" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="U1" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="V1" s="6" t="s">
+      <c r="N1" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="R1" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="S1" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="T1" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="U1" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="V1" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="W1" s="6" t="s">
+      <c r="W1" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="X1" s="6" t="s">
+      <c r="X1" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="Y1" s="6" t="s">
-        <v>41</v>
+      <c r="Y1" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A5" s="6">
+        <v>42984</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix to resolve end point
</commit_message>
<xml_diff>
--- a/Client Avails Upload Template.xlsx
+++ b/Client Avails Upload Template.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="47">
   <si>
     <t>Video Version</t>
   </si>
@@ -129,12 +129,6 @@
     <t>Some sample notes</t>
   </si>
   <si>
-    <t>NR</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
     <t>Required</t>
   </si>
   <si>
@@ -159,13 +153,13 @@
     <t>Title Name</t>
   </si>
   <si>
-    <t>Dummy, Title</t>
-  </si>
-  <si>
-    <t>Dummy, Title1</t>
-  </si>
-  <si>
     <t>Suppress</t>
+  </si>
+  <si>
+    <t>Sample Title 1</t>
+  </si>
+  <si>
+    <t>Sample, Title 2</t>
   </si>
 </sst>
 </file>
@@ -1004,7 +998,7 @@
   <dimension ref="A1:AC4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1032,99 +1026,97 @@
     <col min="24" max="24" width="22.28515625" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="N1" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="C1" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="L1" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="M1" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="N1" s="5" t="s">
+      <c r="O1" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="R1" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="S1" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="T1" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="U1" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="V1" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="W1" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="O1" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="P1" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q1" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="R1" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="S1" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="T1" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="U1" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="V1" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="W1" s="5" t="s">
-        <v>42</v>
-      </c>
       <c r="X1" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="Y1" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="Z1" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="AA1" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="AB1" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>0</v>
@@ -1202,15 +1194,15 @@
         <v>24</v>
       </c>
       <c r="AA2" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="AB2" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B3" s="1">
         <v>6000000001</v>
@@ -1251,44 +1243,30 @@
       <c r="N3" s="4"/>
       <c r="O3" s="4"/>
       <c r="P3" s="4"/>
-      <c r="Q3" s="4">
-        <v>1.99</v>
-      </c>
-      <c r="R3" s="4">
-        <v>1.99</v>
-      </c>
-      <c r="S3" s="2">
-        <v>42522</v>
-      </c>
-      <c r="T3" s="2">
-        <v>42522</v>
-      </c>
+      <c r="Q3" s="4"/>
+      <c r="R3" s="4"/>
+      <c r="S3" s="2"/>
+      <c r="T3" s="2"/>
       <c r="U3" s="1" t="s">
         <v>35</v>
       </c>
       <c r="V3" s="3">
         <v>883316107812</v>
       </c>
-      <c r="W3" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="X3" s="1">
-        <v>5</v>
-      </c>
-      <c r="Y3" s="1" t="s">
-        <v>37</v>
-      </c>
+      <c r="W3" s="1"/>
+      <c r="X3" s="1"/>
+      <c r="Y3" s="1"/>
       <c r="Z3" s="1" t="s">
         <v>33</v>
       </c>
       <c r="AA3" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="AC3" s="5"/>
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B4" s="1">
         <v>6000000002</v>
@@ -1329,39 +1307,25 @@
       <c r="N4" s="4"/>
       <c r="O4" s="4"/>
       <c r="P4" s="4"/>
-      <c r="Q4" s="4">
-        <v>1.99</v>
-      </c>
-      <c r="R4" s="4">
-        <v>1.99</v>
-      </c>
-      <c r="S4" s="2">
-        <v>42522</v>
-      </c>
-      <c r="T4" s="2">
-        <v>42522</v>
-      </c>
+      <c r="Q4" s="4"/>
+      <c r="R4" s="4"/>
+      <c r="S4" s="2"/>
+      <c r="T4" s="2"/>
       <c r="U4" s="1" t="s">
         <v>35</v>
       </c>
       <c r="V4" s="3">
         <v>883316116289</v>
       </c>
-      <c r="W4" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="X4" s="1">
-        <v>5</v>
-      </c>
-      <c r="Y4" s="1" t="s">
-        <v>37</v>
-      </c>
+      <c r="W4" s="1"/>
+      <c r="X4" s="1"/>
+      <c r="Y4" s="1"/>
       <c r="Z4" s="1" t="s">
         <v>33</v>
       </c>
       <c r="AA4" s="1"/>
       <c r="AB4">
-        <v>123</v>
+        <v>123456</v>
       </c>
     </row>
   </sheetData>
@@ -1388,79 +1352,79 @@
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="M1" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="L1" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="M1" s="5" t="s">
+      <c r="N1" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="R1" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="S1" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="T1" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="U1" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="V1" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="N1" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="O1" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="P1" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q1" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="R1" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="S1" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="T1" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="U1" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="V1" s="5" t="s">
-        <v>42</v>
-      </c>
       <c r="W1" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="X1" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="Y1" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">

</xml_diff>